<commit_message>
added analyses to documentation
</commit_message>
<xml_diff>
--- a/Documentation/Project_Structure.xlsx
+++ b/Documentation/Project_Structure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bioinformatics\Projects\WormExp\GitHub\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D9AA6F-705E-493E-881B-8FF8733E7B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20574842-BFD8-4B1A-8BE6-852B429D2383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektstrukturplan" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="162">
   <si>
     <t>Projektstrukturplan</t>
   </si>
@@ -460,9 +460,6 @@
     <t>14.02.: added category epigenetics; 11.10.: eventuell anpassen von Kategorien für Schlagwörter wie "epigenetics"/"microbiome analysis"/etc.</t>
   </si>
   <si>
-    <t>14.02.: first working_package done, second in review at Katja; 15.11.: work in progress; Give list to Katja</t>
-  </si>
-  <si>
     <t>14.02.: no automation, but changed for use for others; 07.10.: including date or other parameter to pre-filter data, etc.</t>
   </si>
   <si>
@@ -487,13 +484,49 @@
     <t>Test database</t>
   </si>
   <si>
-    <t xml:space="preserve">22.02.: generate test sets and test database two times: 1. without updates and 2. with updates; add dataset that includes epigenetics </t>
-  </si>
-  <si>
-    <t>22.02.: check where to upload finished database; make last test after update; 17.02.: check if addition of epigenetics leads to problems, check with test analysis that everything works properly</t>
-  </si>
-  <si>
     <t>07.03.2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24.02.: done; 22.02.: generate test sets and test database two times: 1. without updates and 2. with updates; add dataset that includes epigenetics </t>
+  </si>
+  <si>
+    <t>Proof of Principle</t>
+  </si>
+  <si>
+    <t>11.03.2022</t>
+  </si>
+  <si>
+    <t>13.03.: done</t>
+  </si>
+  <si>
+    <t>references</t>
+  </si>
+  <si>
+    <t>31.07.2022</t>
+  </si>
+  <si>
+    <t>12.03.: references don't work correctly if gene set name is not exactly the same as in reference list -&gt; cannot find some references</t>
+  </si>
+  <si>
+    <t>12.03.; how to do gene enrichment analysis with Bt data sets; Katja feedback summarizing strain data sets; 02.03.: make list with all microbes in database; ask Katja how to upload data</t>
+  </si>
+  <si>
+    <t>12.03.: access server done; 22.02.: check where to upload finished database; make last test after update; 17.02.: check if addition of epigenetics leads to problems, check with test analysis that everything works properly</t>
+  </si>
+  <si>
+    <t>07.03.: transcriptomic list done; 01.03.: second working package WIP; 14.02.: first working_package done, second in review at Katja; 15.11.: work in progress; Give list to Katja</t>
+  </si>
+  <si>
+    <t>Multiple Categories</t>
+  </si>
+  <si>
+    <t>12.03.: WormExp cannot pack data sets in more than one category -&gt; find source file and update</t>
+  </si>
+  <si>
+    <t>Jenny/Yang</t>
+  </si>
+  <si>
+    <t>12.03.: chapter test runs ongoing</t>
   </si>
 </sst>
 </file>
@@ -761,7 +794,23 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -787,14 +836,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>101061</xdr:colOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>136920</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>157296</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>103991</xdr:colOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>139850</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>163158</xdr:rowOff>
     </xdr:to>
@@ -811,7 +860,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12391673" y="748967"/>
+          <a:off x="12660614" y="748967"/>
           <a:ext cx="2930" cy="5806026"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1349,7 +1398,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ26"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -1769,7 +1818,7 @@
         <v>73</v>
       </c>
       <c r="D15" s="41" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="20"/>
@@ -1812,7 +1861,7 @@
         <v>71</v>
       </c>
       <c r="D16" s="41" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="20"/>
@@ -1855,7 +1904,7 @@
         <v>71</v>
       </c>
       <c r="D17" s="41" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="20"/>
@@ -1898,7 +1947,7 @@
         <v>124</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="35"/>
@@ -2021,7 +2070,7 @@
         <v>94</v>
       </c>
       <c r="D21" s="41" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="20"/>
@@ -2187,7 +2236,7 @@
         <v>92</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
@@ -2286,10 +2335,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C350AE8-6BD8-4071-BE8D-EB446D52B86B}">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2297,6 +2346,7 @@
     <col min="2" max="2" width="28.21875" customWidth="1"/>
     <col min="3" max="3" width="26.21875" customWidth="1"/>
     <col min="4" max="4" width="41.21875" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.35">
@@ -2337,57 +2387,57 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B7" s="38" t="s">
-        <v>105</v>
-      </c>
-      <c r="C7" s="39" t="s">
+      <c r="B7" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B8" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="C8" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="40" t="s">
-        <v>140</v>
-      </c>
-      <c r="E7" s="38" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B8" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="33" t="s">
-        <v>138</v>
-      </c>
-      <c r="E8" s="11"/>
-    </row>
-    <row r="9" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D8" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="E8" s="14"/>
+    </row>
+    <row r="9" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="B9" s="9" t="s">
-        <v>147</v>
+        <v>21</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="9" t="s">
-        <v>21</v>
+        <v>158</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>45</v>
+        <v>153</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>32</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -2404,109 +2454,111 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B12" s="9" t="s">
-        <v>29</v>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="14" t="s">
+        <v>133</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>139</v>
+        <v>45</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>161</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B13" s="38" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="C13" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="38" t="s">
+      <c r="D13" s="40" t="s">
+        <v>139</v>
+      </c>
+      <c r="E13" s="38" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B14" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="E14" s="11"/>
+    </row>
+    <row r="15" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B15" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B16" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B17" s="38" t="s">
+        <v>128</v>
+      </c>
+      <c r="C17" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="38" t="s">
         <v>137</v>
       </c>
-      <c r="E13" s="38" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B14" s="9" t="s">
+      <c r="E17" s="38" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B18" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="11" t="s">
+      <c r="C18" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B19" s="11" t="s">
         <v>130</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B16" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B17" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B18" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="21"/>
-      <c r="E18" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B19" s="11" t="s">
-        <v>134</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>45</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="E19" s="11" t="s">
         <v>32</v>
@@ -2514,13 +2566,13 @@
     </row>
     <row r="20" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B20" s="11" t="s">
-        <v>84</v>
+        <v>131</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="44" t="s">
-        <v>146</v>
+        <v>45</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>145</v>
       </c>
       <c r="E20" s="11" t="s">
         <v>32</v>
@@ -2528,27 +2580,27 @@
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="11" t="s">
-        <v>96</v>
+        <v>132</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="D21" s="32" t="s">
-        <v>100</v>
+        <v>45</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>136</v>
       </c>
       <c r="E21" s="11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B22" s="11" t="s">
-        <v>99</v>
+        <v>134</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D22" s="34" t="s">
-        <v>126</v>
+        <v>45</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>136</v>
       </c>
       <c r="E22" s="11" t="s">
         <v>32</v>
@@ -2556,125 +2608,125 @@
     </row>
     <row r="23" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B23" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="44" t="s">
+        <v>145</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B24" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B25" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B26" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C26" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="D23" s="33" t="s">
+      <c r="D26" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="E23" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B24" s="11" t="s">
+      <c r="E26" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B27" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C27" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="D24" s="33" t="s">
+      <c r="D27" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="E24" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="B25" s="38" t="s">
+      <c r="E27" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="B28" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="C25" s="39" t="s">
+      <c r="C28" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="40" t="s">
+      <c r="D28" s="40" t="s">
         <v>113</v>
       </c>
-      <c r="E25" s="38" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B26" s="11" t="s">
+      <c r="E28" s="38" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B29" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C29" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="33" t="s">
+      <c r="D29" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="E26" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B27" s="38" t="s">
+      <c r="E29" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B30" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="C27" s="39" t="s">
+      <c r="C30" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="D27" s="40" t="s">
+      <c r="D30" s="40" t="s">
         <v>110</v>
       </c>
-      <c r="E27" s="38" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B28" s="11" t="s">
+      <c r="E30" s="38" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B31" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C31" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="D28" s="32" t="s">
+      <c r="D31" s="32" t="s">
         <v>102</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B29" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="D29" s="32" t="s">
-        <v>97</v>
-      </c>
-      <c r="E29" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="B30" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B31" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>35</v>
       </c>
       <c r="E31" s="11" t="s">
         <v>32</v>
@@ -2682,190 +2734,232 @@
     </row>
     <row r="32" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B32" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D32" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="B33" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B34" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B35" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C35" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="D35" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="E35" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B33" s="38" t="s">
+    <row r="36" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B36" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="C33" s="39" t="s">
+      <c r="C36" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="D33" s="38" t="s">
+      <c r="D36" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="E33" s="38" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B34" s="11" t="s">
+      <c r="E36" s="38" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B37" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C37" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D34" s="11" t="s">
+      <c r="D37" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="E34" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B35" s="11" t="s">
+      <c r="E37" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B38" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C38" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D35" s="11" t="s">
+      <c r="D38" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="E35" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B36" s="38" t="s">
+      <c r="E38" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B39" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="C36" s="39" t="s">
+      <c r="C39" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="D36" s="38" t="s">
+      <c r="D39" s="38" t="s">
         <v>127</v>
       </c>
-      <c r="E36" s="38" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B37" s="11" t="s">
+      <c r="E39" s="38" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B40" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C40" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D37" s="32" t="s">
+      <c r="D40" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="E37" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B38" s="11" t="s">
+      <c r="E40" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B41" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="C41" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D38" s="11" t="s">
+      <c r="D41" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E38" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B39" s="11" t="s">
+      <c r="E41" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B42" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C39" s="12" t="s">
+      <c r="C42" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D39" s="11" t="s">
+      <c r="D42" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="E39" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="B40" s="11" t="s">
+      <c r="E42" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="B43" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C40" s="12" t="s">
+      <c r="C43" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D40" s="11" t="s">
+      <c r="D43" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="E40" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B41" s="38" t="s">
+      <c r="E43" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B44" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="C41" s="39" t="s">
+      <c r="C44" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="D41" s="38" t="s">
+      <c r="D44" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="E41" s="38" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="B42" s="11" t="s">
+      <c r="E44" s="38" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="B45" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C42" s="12" t="s">
+      <c r="C45" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D42" s="11" t="s">
+      <c r="D45" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="E42" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B43" s="11" t="s">
+      <c r="E45" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B46" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="C43" s="12" t="s">
+      <c r="C46" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D43" s="34" t="s">
+      <c r="D46" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="E43" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B44" s="11" t="s">
+      <c r="E46" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B47" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="C44" s="12" t="s">
+      <c r="C47" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D44" s="34" t="s">
+      <c r="D47" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="E44" s="11" t="s">
+      <c r="E47" s="11" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A6:G44" xr:uid="{2C350AE8-6BD8-4071-BE8D-EB446D52B86B}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:G44">
-      <sortCondition sortBy="cellColor" ref="B6:B44" dxfId="0"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:G47">
+      <sortCondition sortBy="cellColor" ref="B6:B44" dxfId="1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added codeblock Yang and new references
</commit_message>
<xml_diff>
--- a/Documentation/Project_Structure.xlsx
+++ b/Documentation/Project_Structure.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bioinformatics\Projects\WormExp\GitHub\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20574842-BFD8-4B1A-8BE6-852B429D2383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F99C4970-222F-44C2-843C-37BA1E19AE85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="173">
   <si>
     <t>Projektstrukturplan</t>
   </si>
@@ -213,9 +213,6 @@
     <t>Transcriptomics data</t>
   </si>
   <si>
-    <t>Optimization</t>
-  </si>
-  <si>
     <t>Goals (SMART)</t>
   </si>
   <si>
@@ -252,9 +249,6 @@
     <t>30.09.21</t>
   </si>
   <si>
-    <t>Saving milestones on GitHub</t>
-  </si>
-  <si>
     <t>31.12.21</t>
   </si>
   <si>
@@ -313,12 +307,6 @@
   </si>
   <si>
     <t>27.09.2021</t>
-  </si>
-  <si>
-    <t>Pilot Study</t>
-  </si>
-  <si>
-    <t>31.03.22</t>
   </si>
   <si>
     <t>31.02.22</t>
@@ -418,9 +406,6 @@
     <t>15.03.22</t>
   </si>
   <si>
-    <t>Create GSE script version for direct use</t>
-  </si>
-  <si>
     <t>20.01.: done</t>
   </si>
   <si>
@@ -463,9 +448,6 @@
     <t>14.02.: no automation, but changed for use for others; 07.10.: including date or other parameter to pre-filter data, etc.</t>
   </si>
   <si>
-    <t>14.02.: waiting for working package 02; 10.01.: update after first review</t>
-  </si>
-  <si>
     <t>14.02.: done; 10.01.: first draft done, waiting for review; 15:11.: work in progress</t>
   </si>
   <si>
@@ -527,6 +509,57 @@
   </si>
   <si>
     <t>12.03.: chapter test runs ongoing</t>
+  </si>
+  <si>
+    <t>April</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>31.03.: done; 14.02.: waiting for working package 02; 10.01.: update after first review</t>
+  </si>
+  <si>
+    <t>31.07.22</t>
+  </si>
+  <si>
+    <t>Manage Github</t>
+  </si>
+  <si>
+    <t>20.07.22</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>Fix References</t>
+  </si>
+  <si>
+    <t>Test Runs locally</t>
+  </si>
+  <si>
+    <t>31.05.22</t>
+  </si>
+  <si>
+    <t>Update website text</t>
+  </si>
+  <si>
+    <t>Incorporate code changes</t>
+  </si>
+  <si>
+    <t>15.07.22</t>
+  </si>
+  <si>
+    <t>Pilot Study/Test Runs online</t>
+  </si>
+  <si>
+    <t>05.05.: created and regularly updated</t>
   </si>
 </sst>
 </file>
@@ -536,7 +569,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -563,6 +596,13 @@
     </font>
     <font>
       <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -626,7 +666,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -662,11 +702,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -717,9 +795,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -737,9 +812,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -787,30 +859,51 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="8" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -836,16 +929,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>136920</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>157296</xdr:rowOff>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>158691</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>168182</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>139850</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>163158</xdr:rowOff>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>161621</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>174043</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -860,8 +953,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12660614" y="748967"/>
-          <a:ext cx="2930" cy="5806026"/>
+          <a:off x="14418977" y="951953"/>
+          <a:ext cx="2930" cy="5905919"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -952,23 +1045,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>35</xdr:col>
-      <xdr:colOff>56029</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>33168</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>1963</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>108815</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>61284</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>38423</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>14837</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>293366</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Isosceles Triangle 6">
+        <xdr:cNvPr id="24" name="Isosceles Triangle 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCC54C43-B266-4900-97C4-A459ACC8DCD4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9EA00F5-5AF6-4A0C-B106-7C0AC091DE8B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -976,8 +1069,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13278970" y="4954792"/>
-          <a:ext cx="238338" cy="184549"/>
+          <a:off x="10660998" y="3416791"/>
+          <a:ext cx="245957" cy="184551"/>
         </a:xfrm>
         <a:prstGeom prst="triangle">
           <a:avLst/>
@@ -1012,23 +1105,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>35</xdr:col>
-      <xdr:colOff>46787</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>1238</xdr:rowOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>69198</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>42218</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>59661</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>6494</xdr:rowOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>71186</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>226769</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="23" name="Isosceles Triangle 22">
+        <xdr:cNvPr id="32" name="Isosceles Triangle 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{896F49CE-6379-4DCC-95DA-F49F7F6CC624}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20F3AE0A-E244-47B6-AEFF-59E6DE4D5200}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1036,8 +1129,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13269728" y="3847097"/>
-          <a:ext cx="245957" cy="184550"/>
+          <a:off x="13055855" y="4505361"/>
+          <a:ext cx="241474" cy="184551"/>
         </a:xfrm>
         <a:prstGeom prst="triangle">
           <a:avLst/>
@@ -1072,23 +1165,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>1963</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>108815</xdr:rowOff>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>90968</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>140188</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>14837</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>293366</xdr:rowOff>
+      <xdr:col>52</xdr:col>
+      <xdr:colOff>103842</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>139682</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="24" name="Isosceles Triangle 23">
+        <xdr:cNvPr id="33" name="Isosceles Triangle 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9EA00F5-5AF6-4A0C-B106-7C0AC091DE8B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D43B2090-B411-49E5-B843-4078E305952B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1096,8 +1189,128 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10660998" y="3416791"/>
-          <a:ext cx="245957" cy="184551"/>
+          <a:off x="16985597" y="7183245"/>
+          <a:ext cx="241474" cy="184551"/>
+        </a:xfrm>
+        <a:prstGeom prst="triangle">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1800"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>47425</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>63987</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>60299</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>63481</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="34" name="Isosceles Triangle 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10919730-2E23-4628-B263-C2C29CCCD9EE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16713454" y="5441530"/>
+          <a:ext cx="241474" cy="184551"/>
+        </a:xfrm>
+        <a:prstGeom prst="triangle">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1800"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>90968</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>357902</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>103842</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>172339</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="35" name="Isosceles Triangle 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{595BDD34-D0A2-47A3-A8CC-9EF1F2A08D83}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12370054" y="7030845"/>
+          <a:ext cx="241474" cy="184551"/>
         </a:xfrm>
         <a:prstGeom prst="triangle">
           <a:avLst/>
@@ -1396,73 +1609,90 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AJ26"/>
+  <dimension ref="A1:AZ29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="BA20" sqref="BA20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="35.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.21875" customWidth="1"/>
     <col min="4" max="4" width="30.6640625" customWidth="1"/>
     <col min="5" max="32" width="3.33203125" customWidth="1"/>
     <col min="33" max="36" width="3.44140625" customWidth="1"/>
+    <col min="37" max="52" width="3.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:52" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="E6" s="46">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="E6" s="45">
         <v>2021</v>
       </c>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="46"/>
-      <c r="K6" s="46"/>
-      <c r="L6" s="46"/>
-      <c r="M6" s="46"/>
-      <c r="N6" s="46"/>
-      <c r="O6" s="46"/>
-      <c r="P6" s="46"/>
-      <c r="Q6" s="46"/>
-      <c r="R6" s="46"/>
-      <c r="S6" s="46"/>
-      <c r="T6" s="46"/>
-      <c r="U6" s="46"/>
-      <c r="V6" s="46"/>
-      <c r="W6" s="46"/>
-      <c r="X6" s="46"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="45"/>
+      <c r="K6" s="45"/>
+      <c r="L6" s="45"/>
+      <c r="M6" s="45"/>
+      <c r="N6" s="45"/>
+      <c r="O6" s="45"/>
+      <c r="P6" s="45"/>
+      <c r="Q6" s="45"/>
+      <c r="R6" s="45"/>
+      <c r="S6" s="45"/>
+      <c r="T6" s="45"/>
+      <c r="U6" s="45"/>
+      <c r="V6" s="45"/>
+      <c r="W6" s="45"/>
+      <c r="X6" s="45"/>
       <c r="Y6" s="46">
         <v>2022</v>
       </c>
-      <c r="Z6" s="46"/>
-      <c r="AA6" s="46"/>
-      <c r="AB6" s="46"/>
-      <c r="AC6" s="46"/>
-      <c r="AD6" s="46"/>
-      <c r="AE6" s="46"/>
-      <c r="AF6" s="46"/>
-      <c r="AG6" s="46"/>
-      <c r="AH6" s="46"/>
-      <c r="AI6" s="46"/>
-      <c r="AJ6" s="46"/>
-    </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="Z6" s="47"/>
+      <c r="AA6" s="47"/>
+      <c r="AB6" s="47"/>
+      <c r="AC6" s="47"/>
+      <c r="AD6" s="47"/>
+      <c r="AE6" s="47"/>
+      <c r="AF6" s="47"/>
+      <c r="AG6" s="47"/>
+      <c r="AH6" s="47"/>
+      <c r="AI6" s="47"/>
+      <c r="AJ6" s="47"/>
+      <c r="AK6" s="47"/>
+      <c r="AL6" s="47"/>
+      <c r="AM6" s="47"/>
+      <c r="AN6" s="47"/>
+      <c r="AO6" s="47"/>
+      <c r="AP6" s="47"/>
+      <c r="AQ6" s="47"/>
+      <c r="AR6" s="47"/>
+      <c r="AS6" s="47"/>
+      <c r="AT6" s="47"/>
+      <c r="AU6" s="47"/>
+      <c r="AV6" s="47"/>
+      <c r="AW6" s="47"/>
+      <c r="AX6" s="47"/>
+      <c r="AY6" s="47"/>
+      <c r="AZ6" s="48"/>
+    </row>
+    <row r="7" spans="1:52" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
         <v>2</v>
       </c>
@@ -1472,61 +1702,85 @@
       <c r="D7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="45" t="s">
+      <c r="E7" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="45" t="s">
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="J7" s="45"/>
-      <c r="K7" s="45"/>
-      <c r="L7" s="45"/>
-      <c r="M7" s="45" t="s">
+      <c r="J7" s="44"/>
+      <c r="K7" s="44"/>
+      <c r="L7" s="44"/>
+      <c r="M7" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="N7" s="45"/>
-      <c r="O7" s="45"/>
-      <c r="P7" s="45"/>
-      <c r="Q7" s="45" t="s">
+      <c r="N7" s="44"/>
+      <c r="O7" s="44"/>
+      <c r="P7" s="44"/>
+      <c r="Q7" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="R7" s="45"/>
-      <c r="S7" s="45"/>
-      <c r="T7" s="45"/>
-      <c r="U7" s="45" t="s">
+      <c r="R7" s="44"/>
+      <c r="S7" s="44"/>
+      <c r="T7" s="44"/>
+      <c r="U7" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="V7" s="45"/>
-      <c r="W7" s="45"/>
-      <c r="X7" s="45"/>
-      <c r="Y7" s="45" t="s">
+      <c r="V7" s="44"/>
+      <c r="W7" s="44"/>
+      <c r="X7" s="44"/>
+      <c r="Y7" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="Z7" s="45"/>
-      <c r="AA7" s="45"/>
-      <c r="AB7" s="45"/>
-      <c r="AC7" s="45" t="s">
+      <c r="Z7" s="44"/>
+      <c r="AA7" s="44"/>
+      <c r="AB7" s="44"/>
+      <c r="AC7" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="AD7" s="45"/>
-      <c r="AE7" s="45"/>
-      <c r="AF7" s="45"/>
-      <c r="AG7" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="AH7" s="45"/>
-      <c r="AI7" s="45"/>
-      <c r="AJ7" s="45"/>
-    </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="B8" s="25" t="s">
+      <c r="AD7" s="44"/>
+      <c r="AE7" s="44"/>
+      <c r="AF7" s="44"/>
+      <c r="AG7" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH7" s="44"/>
+      <c r="AI7" s="44"/>
+      <c r="AJ7" s="44"/>
+      <c r="AK7" s="44" t="s">
+        <v>156</v>
+      </c>
+      <c r="AL7" s="44"/>
+      <c r="AM7" s="44"/>
+      <c r="AN7" s="44"/>
+      <c r="AO7" s="44" t="s">
+        <v>157</v>
+      </c>
+      <c r="AP7" s="44"/>
+      <c r="AQ7" s="44"/>
+      <c r="AR7" s="44"/>
+      <c r="AS7" s="44" t="s">
+        <v>158</v>
+      </c>
+      <c r="AT7" s="44"/>
+      <c r="AU7" s="44"/>
+      <c r="AV7" s="44"/>
+      <c r="AW7" s="44" t="s">
+        <v>159</v>
+      </c>
+      <c r="AX7" s="44"/>
+      <c r="AY7" s="44"/>
+      <c r="AZ7" s="44"/>
+    </row>
+    <row r="8" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="B8" s="24" t="s">
         <v>55</v>
       </c>
       <c r="C8" s="6"/>
-      <c r="D8" s="23"/>
+      <c r="D8" s="22"/>
       <c r="E8" s="20"/>
       <c r="F8" s="20"/>
       <c r="G8" s="20"/>
@@ -1559,25 +1813,41 @@
       <c r="AH8" s="20"/>
       <c r="AI8" s="20"/>
       <c r="AJ8" s="20"/>
-    </row>
-    <row r="9" spans="1:36" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B9" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="D9" s="42" t="s">
-        <v>95</v>
-      </c>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="30"/>
+      <c r="AK8" s="43"/>
+      <c r="AL8" s="43"/>
+      <c r="AM8" s="43"/>
+      <c r="AN8" s="43"/>
+      <c r="AO8" s="43"/>
+      <c r="AP8" s="43"/>
+      <c r="AQ8" s="43"/>
+      <c r="AR8" s="43"/>
+      <c r="AS8" s="43"/>
+      <c r="AT8" s="43"/>
+      <c r="AU8" s="43"/>
+      <c r="AV8" s="43"/>
+      <c r="AW8" s="43"/>
+      <c r="AX8" s="43"/>
+      <c r="AY8" s="43"/>
+      <c r="AZ8" s="43"/>
+    </row>
+    <row r="9" spans="1:52" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B9" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
       <c r="M9" s="20"/>
       <c r="N9" s="20"/>
       <c r="O9" s="20"/>
@@ -1602,25 +1872,41 @@
       <c r="AH9" s="20"/>
       <c r="AI9" s="20"/>
       <c r="AJ9" s="20"/>
-    </row>
-    <row r="10" spans="1:36" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B10" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="D10" s="42" t="s">
-        <v>95</v>
-      </c>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="30"/>
-      <c r="L10" s="30"/>
+      <c r="AK9" s="43"/>
+      <c r="AL9" s="43"/>
+      <c r="AM9" s="43"/>
+      <c r="AN9" s="43"/>
+      <c r="AO9" s="43"/>
+      <c r="AP9" s="43"/>
+      <c r="AQ9" s="43"/>
+      <c r="AR9" s="43"/>
+      <c r="AS9" s="43"/>
+      <c r="AT9" s="43"/>
+      <c r="AU9" s="43"/>
+      <c r="AV9" s="43"/>
+      <c r="AW9" s="43"/>
+      <c r="AX9" s="43"/>
+      <c r="AY9" s="43"/>
+      <c r="AZ9" s="43"/>
+    </row>
+    <row r="10" spans="1:52" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B10" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
       <c r="M10" s="20"/>
       <c r="N10" s="20"/>
       <c r="O10" s="20"/>
@@ -1645,25 +1931,41 @@
       <c r="AH10" s="20"/>
       <c r="AI10" s="20"/>
       <c r="AJ10" s="20"/>
-    </row>
-    <row r="11" spans="1:36" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11" s="42" t="s">
-        <v>95</v>
-      </c>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="30"/>
-      <c r="L11" s="30"/>
+      <c r="AK10" s="43"/>
+      <c r="AL10" s="43"/>
+      <c r="AM10" s="43"/>
+      <c r="AN10" s="43"/>
+      <c r="AO10" s="43"/>
+      <c r="AP10" s="43"/>
+      <c r="AQ10" s="43"/>
+      <c r="AR10" s="43"/>
+      <c r="AS10" s="43"/>
+      <c r="AT10" s="43"/>
+      <c r="AU10" s="43"/>
+      <c r="AV10" s="43"/>
+      <c r="AW10" s="43"/>
+      <c r="AX10" s="43"/>
+      <c r="AY10" s="43"/>
+      <c r="AZ10" s="43"/>
+    </row>
+    <row r="11" spans="1:52" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B11" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
       <c r="M11" s="20"/>
       <c r="N11" s="20"/>
       <c r="O11" s="20"/>
@@ -1688,14 +1990,30 @@
       <c r="AH11" s="20"/>
       <c r="AI11" s="20"/>
       <c r="AJ11" s="20"/>
-    </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="B12" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="20"/>
+      <c r="AK11" s="43"/>
+      <c r="AL11" s="43"/>
+      <c r="AM11" s="43"/>
+      <c r="AN11" s="43"/>
+      <c r="AO11" s="43"/>
+      <c r="AP11" s="43"/>
+      <c r="AQ11" s="43"/>
+      <c r="AR11" s="43"/>
+      <c r="AS11" s="43"/>
+      <c r="AT11" s="43"/>
+      <c r="AU11" s="43"/>
+      <c r="AV11" s="43"/>
+      <c r="AW11" s="43"/>
+      <c r="AX11" s="43"/>
+      <c r="AY11" s="43"/>
+      <c r="AZ11" s="43"/>
+    </row>
+    <row r="12" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="B12" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="27"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="4"/>
       <c r="F12" s="20"/>
       <c r="G12" s="20"/>
       <c r="H12" s="20"/>
@@ -1727,13 +2045,33 @@
       <c r="AH12" s="20"/>
       <c r="AI12" s="20"/>
       <c r="AJ12" s="20"/>
-    </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="B13" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" s="28"/>
-      <c r="D13" s="23"/>
+      <c r="AK12" s="43"/>
+      <c r="AL12" s="43"/>
+      <c r="AM12" s="43"/>
+      <c r="AN12" s="43"/>
+      <c r="AO12" s="43"/>
+      <c r="AP12" s="43"/>
+      <c r="AQ12" s="43"/>
+      <c r="AR12" s="43"/>
+      <c r="AS12" s="43"/>
+      <c r="AT12" s="43"/>
+      <c r="AU12" s="43"/>
+      <c r="AV12" s="43"/>
+      <c r="AW12" s="43"/>
+      <c r="AX12" s="43"/>
+      <c r="AY12" s="43"/>
+      <c r="AZ12" s="43"/>
+    </row>
+    <row r="13" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="B13" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="39" t="s">
+        <v>35</v>
+      </c>
       <c r="E13" s="4"/>
       <c r="F13" s="20"/>
       <c r="G13" s="20"/>
@@ -1742,7 +2080,7 @@
       <c r="J13" s="20"/>
       <c r="K13" s="20"/>
       <c r="L13" s="20"/>
-      <c r="M13" s="20"/>
+      <c r="M13" s="28"/>
       <c r="N13" s="20"/>
       <c r="O13" s="20"/>
       <c r="P13" s="20"/>
@@ -1766,16 +2104,32 @@
       <c r="AH13" s="20"/>
       <c r="AI13" s="20"/>
       <c r="AJ13" s="20"/>
-    </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="B14" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="C14" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="D14" s="41" t="s">
-        <v>35</v>
+      <c r="AK13" s="43"/>
+      <c r="AL13" s="43"/>
+      <c r="AM13" s="43"/>
+      <c r="AN13" s="43"/>
+      <c r="AO13" s="43"/>
+      <c r="AP13" s="43"/>
+      <c r="AQ13" s="43"/>
+      <c r="AR13" s="43"/>
+      <c r="AS13" s="43"/>
+      <c r="AT13" s="43"/>
+      <c r="AU13" s="43"/>
+      <c r="AV13" s="43"/>
+      <c r="AW13" s="43"/>
+      <c r="AX13" s="43"/>
+      <c r="AY13" s="43"/>
+      <c r="AZ13" s="43"/>
+    </row>
+    <row r="14" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="B14" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="39" t="s">
+        <v>136</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="20"/>
@@ -1785,10 +2139,10 @@
       <c r="J14" s="20"/>
       <c r="K14" s="20"/>
       <c r="L14" s="20"/>
-      <c r="M14" s="30"/>
-      <c r="N14" s="20"/>
-      <c r="O14" s="20"/>
-      <c r="P14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="28"/>
+      <c r="P14" s="28"/>
       <c r="Q14" s="20"/>
       <c r="R14" s="20"/>
       <c r="S14" s="20"/>
@@ -1809,18 +2163,34 @@
       <c r="AH14" s="20"/>
       <c r="AI14" s="20"/>
       <c r="AJ14" s="20"/>
-    </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="B15" s="27" t="s">
-        <v>115</v>
-      </c>
-      <c r="C15" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="D15" s="41" t="s">
-        <v>142</v>
-      </c>
-      <c r="E15" s="4"/>
+      <c r="AK14" s="43"/>
+      <c r="AL14" s="43"/>
+      <c r="AM14" s="43"/>
+      <c r="AN14" s="43"/>
+      <c r="AO14" s="43"/>
+      <c r="AP14" s="43"/>
+      <c r="AQ14" s="43"/>
+      <c r="AR14" s="43"/>
+      <c r="AS14" s="43"/>
+      <c r="AT14" s="43"/>
+      <c r="AU14" s="43"/>
+      <c r="AV14" s="43"/>
+      <c r="AW14" s="43"/>
+      <c r="AX14" s="43"/>
+      <c r="AY14" s="43"/>
+      <c r="AZ14" s="43"/>
+    </row>
+    <row r="15" spans="1:52" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B15" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="39" t="s">
+        <v>135</v>
+      </c>
+      <c r="E15" s="2"/>
       <c r="F15" s="20"/>
       <c r="G15" s="20"/>
       <c r="H15" s="20"/>
@@ -1829,18 +2199,18 @@
       <c r="K15" s="20"/>
       <c r="L15" s="20"/>
       <c r="M15" s="20"/>
-      <c r="N15" s="30"/>
-      <c r="O15" s="30"/>
-      <c r="P15" s="30"/>
-      <c r="Q15" s="20"/>
-      <c r="R15" s="20"/>
-      <c r="S15" s="20"/>
-      <c r="T15" s="20"/>
-      <c r="U15" s="20"/>
-      <c r="V15" s="20"/>
-      <c r="W15" s="20"/>
-      <c r="X15" s="20"/>
-      <c r="Y15" s="20"/>
+      <c r="N15" s="20"/>
+      <c r="O15" s="20"/>
+      <c r="P15" s="28"/>
+      <c r="Q15" s="28"/>
+      <c r="R15" s="28"/>
+      <c r="S15" s="28"/>
+      <c r="T15" s="28"/>
+      <c r="U15" s="28"/>
+      <c r="V15" s="28"/>
+      <c r="W15" s="28"/>
+      <c r="X15" s="28"/>
+      <c r="Y15" s="28"/>
       <c r="Z15" s="20"/>
       <c r="AA15" s="20"/>
       <c r="AB15" s="20"/>
@@ -1852,16 +2222,32 @@
       <c r="AH15" s="20"/>
       <c r="AI15" s="20"/>
       <c r="AJ15" s="20"/>
-    </row>
-    <row r="16" spans="1:36" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B16" s="27" t="s">
+      <c r="AK15" s="43"/>
+      <c r="AL15" s="43"/>
+      <c r="AM15" s="43"/>
+      <c r="AN15" s="43"/>
+      <c r="AO15" s="43"/>
+      <c r="AP15" s="43"/>
+      <c r="AQ15" s="43"/>
+      <c r="AR15" s="43"/>
+      <c r="AS15" s="43"/>
+      <c r="AT15" s="43"/>
+      <c r="AU15" s="43"/>
+      <c r="AV15" s="43"/>
+      <c r="AW15" s="43"/>
+      <c r="AX15" s="43"/>
+      <c r="AY15" s="43"/>
+      <c r="AZ15" s="43"/>
+    </row>
+    <row r="16" spans="1:52" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B16" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="D16" s="41" t="s">
-        <v>141</v>
+      <c r="C16" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="39" t="s">
+        <v>135</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="20"/>
@@ -1874,16 +2260,16 @@
       <c r="M16" s="20"/>
       <c r="N16" s="20"/>
       <c r="O16" s="20"/>
-      <c r="P16" s="30"/>
-      <c r="Q16" s="30"/>
-      <c r="R16" s="30"/>
-      <c r="S16" s="30"/>
-      <c r="T16" s="30"/>
-      <c r="U16" s="30"/>
-      <c r="V16" s="30"/>
-      <c r="W16" s="30"/>
-      <c r="X16" s="30"/>
-      <c r="Y16" s="30"/>
+      <c r="P16" s="20"/>
+      <c r="Q16" s="28"/>
+      <c r="R16" s="28"/>
+      <c r="S16" s="28"/>
+      <c r="T16" s="28"/>
+      <c r="U16" s="28"/>
+      <c r="V16" s="28"/>
+      <c r="W16" s="28"/>
+      <c r="X16" s="28"/>
+      <c r="Y16" s="28"/>
       <c r="Z16" s="20"/>
       <c r="AA16" s="20"/>
       <c r="AB16" s="20"/>
@@ -1895,101 +2281,145 @@
       <c r="AH16" s="20"/>
       <c r="AI16" s="20"/>
       <c r="AJ16" s="20"/>
-    </row>
-    <row r="17" spans="2:36" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B17" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="D17" s="41" t="s">
-        <v>141</v>
+      <c r="AK16" s="43"/>
+      <c r="AL16" s="43"/>
+      <c r="AM16" s="43"/>
+      <c r="AN16" s="43"/>
+      <c r="AO16" s="43"/>
+      <c r="AP16" s="43"/>
+      <c r="AQ16" s="43"/>
+      <c r="AR16" s="43"/>
+      <c r="AS16" s="43"/>
+      <c r="AT16" s="43"/>
+      <c r="AU16" s="43"/>
+      <c r="AV16" s="43"/>
+      <c r="AW16" s="43"/>
+      <c r="AX16" s="43"/>
+      <c r="AY16" s="43"/>
+      <c r="AZ16" s="43"/>
+    </row>
+    <row r="17" spans="2:52" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B17" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D17" s="39" t="s">
+        <v>160</v>
       </c>
       <c r="E17" s="2"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="20"/>
-      <c r="M17" s="20"/>
-      <c r="N17" s="20"/>
-      <c r="O17" s="20"/>
-      <c r="P17" s="20"/>
-      <c r="Q17" s="30"/>
-      <c r="R17" s="30"/>
-      <c r="S17" s="30"/>
-      <c r="T17" s="30"/>
-      <c r="U17" s="30"/>
-      <c r="V17" s="30"/>
-      <c r="W17" s="30"/>
-      <c r="X17" s="30"/>
-      <c r="Y17" s="30"/>
-      <c r="Z17" s="20"/>
-      <c r="AA17" s="20"/>
-      <c r="AB17" s="20"/>
-      <c r="AC17" s="20"/>
-      <c r="AD17" s="20"/>
-      <c r="AE17" s="20"/>
-      <c r="AF17" s="20"/>
-      <c r="AG17" s="20"/>
-      <c r="AH17" s="20"/>
-      <c r="AI17" s="20"/>
-      <c r="AJ17" s="20"/>
-    </row>
-    <row r="18" spans="2:36" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B18" s="27" t="s">
-        <v>123</v>
-      </c>
-      <c r="C18" s="24" t="s">
-        <v>124</v>
-      </c>
-      <c r="D18" s="23" t="s">
-        <v>140</v>
-      </c>
+      <c r="F17" s="33"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
+      <c r="K17" s="33"/>
+      <c r="L17" s="33"/>
+      <c r="M17" s="33"/>
+      <c r="N17" s="33"/>
+      <c r="O17" s="33"/>
+      <c r="P17" s="33"/>
+      <c r="Q17" s="33"/>
+      <c r="R17" s="33"/>
+      <c r="S17" s="33"/>
+      <c r="T17" s="33"/>
+      <c r="U17" s="33"/>
+      <c r="V17" s="33"/>
+      <c r="W17" s="33"/>
+      <c r="X17" s="33"/>
+      <c r="Y17" s="33"/>
+      <c r="Z17" s="33"/>
+      <c r="AA17" s="33"/>
+      <c r="AB17" s="28"/>
+      <c r="AC17" s="28"/>
+      <c r="AD17" s="28"/>
+      <c r="AE17" s="28"/>
+      <c r="AF17" s="28"/>
+      <c r="AG17" s="28"/>
+      <c r="AH17" s="28"/>
+      <c r="AI17" s="28"/>
+      <c r="AJ17" s="43"/>
+      <c r="AK17" s="43"/>
+      <c r="AL17" s="43"/>
+      <c r="AM17" s="43"/>
+      <c r="AN17" s="43"/>
+      <c r="AO17" s="43"/>
+      <c r="AP17" s="43"/>
+      <c r="AQ17" s="43"/>
+      <c r="AR17" s="43"/>
+      <c r="AS17" s="43"/>
+      <c r="AT17" s="43"/>
+      <c r="AU17" s="43"/>
+      <c r="AV17" s="43"/>
+      <c r="AW17" s="43"/>
+      <c r="AX17" s="43"/>
+      <c r="AY17" s="43"/>
+      <c r="AZ17" s="43"/>
+    </row>
+    <row r="18" spans="2:52" x14ac:dyDescent="0.3">
+      <c r="B18" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="C18" s="27"/>
+      <c r="D18" s="22"/>
       <c r="E18" s="2"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="35"/>
-      <c r="L18" s="35"/>
-      <c r="M18" s="35"/>
-      <c r="N18" s="35"/>
-      <c r="O18" s="35"/>
-      <c r="P18" s="35"/>
-      <c r="Q18" s="35"/>
-      <c r="R18" s="35"/>
-      <c r="S18" s="35"/>
-      <c r="T18" s="35"/>
-      <c r="U18" s="35"/>
-      <c r="V18" s="35"/>
-      <c r="W18" s="35"/>
-      <c r="X18" s="35"/>
-      <c r="Y18" s="35"/>
-      <c r="Z18" s="35"/>
-      <c r="AA18" s="35"/>
-      <c r="AB18" s="30"/>
-      <c r="AC18" s="30"/>
-      <c r="AD18" s="30"/>
-      <c r="AE18" s="30"/>
-      <c r="AF18" s="30"/>
-      <c r="AG18" s="30"/>
-      <c r="AH18" s="30"/>
-      <c r="AI18" s="30"/>
-      <c r="AJ18" s="35"/>
-    </row>
-    <row r="19" spans="2:36" x14ac:dyDescent="0.3">
-      <c r="B19" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="D19" s="23"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="20"/>
+      <c r="O18" s="20"/>
+      <c r="P18" s="20"/>
+      <c r="Q18" s="20"/>
+      <c r="R18" s="20"/>
+      <c r="S18" s="20"/>
+      <c r="T18" s="20"/>
+      <c r="U18" s="20"/>
+      <c r="V18" s="20"/>
+      <c r="W18" s="20"/>
+      <c r="X18" s="20"/>
+      <c r="Y18" s="20"/>
+      <c r="Z18" s="20"/>
+      <c r="AA18" s="20"/>
+      <c r="AB18" s="20"/>
+      <c r="AC18" s="20"/>
+      <c r="AD18" s="20"/>
+      <c r="AE18" s="20"/>
+      <c r="AF18" s="20"/>
+      <c r="AG18" s="20"/>
+      <c r="AH18" s="43"/>
+      <c r="AI18" s="43"/>
+      <c r="AJ18" s="43"/>
+      <c r="AK18" s="43"/>
+      <c r="AL18" s="43"/>
+      <c r="AM18" s="43"/>
+      <c r="AN18" s="43"/>
+      <c r="AO18" s="43"/>
+      <c r="AP18" s="43"/>
+      <c r="AQ18" s="43"/>
+      <c r="AR18" s="43"/>
+      <c r="AS18" s="43"/>
+      <c r="AT18" s="43"/>
+      <c r="AU18" s="43"/>
+      <c r="AV18" s="43"/>
+      <c r="AW18" s="43"/>
+      <c r="AX18" s="43"/>
+      <c r="AY18" s="43"/>
+      <c r="AZ18" s="43"/>
+    </row>
+    <row r="19" spans="2:52" x14ac:dyDescent="0.3">
+      <c r="B19" s="26" t="s">
+        <v>165</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="D19" s="22"/>
       <c r="E19" s="2"/>
       <c r="F19" s="20"/>
       <c r="G19" s="20"/>
@@ -2010,199 +2440,279 @@
       <c r="V19" s="20"/>
       <c r="W19" s="20"/>
       <c r="X19" s="20"/>
-      <c r="Y19" s="35"/>
-      <c r="Z19" s="35"/>
-      <c r="AA19" s="35"/>
-      <c r="AB19" s="35"/>
-      <c r="AC19" s="35"/>
-      <c r="AD19" s="35"/>
-      <c r="AE19" s="35"/>
-      <c r="AF19" s="35"/>
-      <c r="AG19" s="35"/>
-      <c r="AH19" s="35"/>
-      <c r="AI19" s="35"/>
-      <c r="AJ19" s="30"/>
-    </row>
-    <row r="20" spans="2:36" x14ac:dyDescent="0.3">
-      <c r="B20" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="C20" s="28"/>
-      <c r="D20" s="23"/>
+      <c r="Y19" s="20"/>
+      <c r="Z19" s="20"/>
+      <c r="AA19" s="20"/>
+      <c r="AB19" s="20"/>
+      <c r="AC19" s="43"/>
+      <c r="AD19" s="43"/>
+      <c r="AE19" s="43"/>
+      <c r="AF19" s="43"/>
+      <c r="AG19" s="43"/>
+      <c r="AH19" s="43"/>
+      <c r="AI19" s="43"/>
+      <c r="AJ19" s="43"/>
+      <c r="AK19" s="43"/>
+      <c r="AL19" s="43"/>
+      <c r="AM19" s="43"/>
+      <c r="AN19" s="28"/>
+      <c r="AO19" s="28"/>
+      <c r="AP19" s="28"/>
+      <c r="AQ19" s="28"/>
+      <c r="AR19" s="28"/>
+      <c r="AS19" s="28"/>
+      <c r="AT19" s="43"/>
+      <c r="AU19" s="43"/>
+      <c r="AV19" s="43"/>
+      <c r="AW19" s="43"/>
+      <c r="AX19" s="43"/>
+      <c r="AY19" s="43"/>
+      <c r="AZ19" s="43"/>
+    </row>
+    <row r="20" spans="2:52" x14ac:dyDescent="0.3">
+      <c r="B20" s="26" t="s">
+        <v>168</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="D20" s="22"/>
       <c r="E20" s="2"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="20"/>
-      <c r="M20" s="20"/>
-      <c r="N20" s="20"/>
-      <c r="O20" s="20"/>
-      <c r="P20" s="20"/>
-      <c r="Q20" s="20"/>
-      <c r="R20" s="20"/>
-      <c r="S20" s="20"/>
-      <c r="T20" s="20"/>
-      <c r="U20" s="20"/>
-      <c r="V20" s="20"/>
-      <c r="W20" s="20"/>
-      <c r="X20" s="20"/>
-      <c r="Y20" s="20"/>
-      <c r="Z20" s="20"/>
-      <c r="AA20" s="20"/>
-      <c r="AB20" s="20"/>
-      <c r="AC20" s="20"/>
-      <c r="AD20" s="20"/>
-      <c r="AE20" s="20"/>
-      <c r="AF20" s="20"/>
-      <c r="AG20" s="20"/>
-      <c r="AH20" s="20"/>
-      <c r="AI20" s="20"/>
-      <c r="AJ20" s="20"/>
-    </row>
-    <row r="21" spans="2:36" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B21" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="C21" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="D21" s="41" t="s">
-        <v>143</v>
-      </c>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="43"/>
+      <c r="J20" s="43"/>
+      <c r="K20" s="43"/>
+      <c r="L20" s="43"/>
+      <c r="M20" s="43"/>
+      <c r="N20" s="43"/>
+      <c r="O20" s="43"/>
+      <c r="P20" s="43"/>
+      <c r="Q20" s="43"/>
+      <c r="R20" s="43"/>
+      <c r="S20" s="43"/>
+      <c r="T20" s="43"/>
+      <c r="U20" s="43"/>
+      <c r="V20" s="43"/>
+      <c r="W20" s="43"/>
+      <c r="X20" s="43"/>
+      <c r="Y20" s="43"/>
+      <c r="Z20" s="43"/>
+      <c r="AA20" s="43"/>
+      <c r="AB20" s="43"/>
+      <c r="AC20" s="43"/>
+      <c r="AD20" s="43"/>
+      <c r="AE20" s="43"/>
+      <c r="AF20" s="43"/>
+      <c r="AG20" s="43"/>
+      <c r="AH20" s="43"/>
+      <c r="AI20" s="43"/>
+      <c r="AJ20" s="43"/>
+      <c r="AK20" s="43"/>
+      <c r="AL20" s="43"/>
+      <c r="AM20" s="43"/>
+      <c r="AN20" s="43"/>
+      <c r="AO20" s="43"/>
+      <c r="AP20" s="43"/>
+      <c r="AQ20" s="43"/>
+      <c r="AR20" s="43"/>
+      <c r="AS20" s="50"/>
+      <c r="AT20" s="43"/>
+      <c r="AU20" s="43"/>
+      <c r="AV20" s="43"/>
+      <c r="AW20" s="43"/>
+      <c r="AX20" s="43"/>
+      <c r="AY20" s="43"/>
+      <c r="AZ20" s="43"/>
+    </row>
+    <row r="21" spans="2:52" x14ac:dyDescent="0.3">
+      <c r="B21" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="D21" s="22"/>
       <c r="E21" s="2"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="30"/>
-      <c r="J21" s="30"/>
-      <c r="K21" s="30"/>
-      <c r="L21" s="30"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="20"/>
-      <c r="O21" s="20"/>
-      <c r="P21" s="20"/>
-      <c r="Q21" s="20"/>
-      <c r="R21" s="20"/>
-      <c r="S21" s="20"/>
-      <c r="T21" s="20"/>
-      <c r="U21" s="20"/>
-      <c r="V21" s="20"/>
-      <c r="W21" s="20"/>
-      <c r="X21" s="20"/>
-      <c r="Y21" s="35"/>
-      <c r="Z21" s="35"/>
-      <c r="AA21" s="35"/>
-      <c r="AB21" s="35"/>
-      <c r="AC21" s="35"/>
-      <c r="AD21" s="20"/>
-      <c r="AE21" s="20"/>
-      <c r="AF21" s="20"/>
-      <c r="AG21" s="20"/>
-      <c r="AH21" s="20"/>
-      <c r="AI21" s="20"/>
-      <c r="AJ21" s="20"/>
-    </row>
-    <row r="22" spans="2:36" x14ac:dyDescent="0.3">
-      <c r="B22" s="36" t="s">
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="43"/>
+      <c r="J21" s="43"/>
+      <c r="K21" s="43"/>
+      <c r="L21" s="43"/>
+      <c r="M21" s="43"/>
+      <c r="N21" s="43"/>
+      <c r="O21" s="43"/>
+      <c r="P21" s="43"/>
+      <c r="Q21" s="43"/>
+      <c r="R21" s="43"/>
+      <c r="S21" s="43"/>
+      <c r="T21" s="43"/>
+      <c r="U21" s="43"/>
+      <c r="V21" s="43"/>
+      <c r="W21" s="43"/>
+      <c r="X21" s="43"/>
+      <c r="Y21" s="43"/>
+      <c r="Z21" s="43"/>
+      <c r="AA21" s="43"/>
+      <c r="AB21" s="43"/>
+      <c r="AC21" s="43"/>
+      <c r="AD21" s="43"/>
+      <c r="AE21" s="43"/>
+      <c r="AF21" s="43"/>
+      <c r="AG21" s="43"/>
+      <c r="AH21" s="43"/>
+      <c r="AI21" s="43"/>
+      <c r="AJ21" s="43"/>
+      <c r="AK21" s="43"/>
+      <c r="AL21" s="43"/>
+      <c r="AM21" s="43"/>
+      <c r="AN21" s="43"/>
+      <c r="AO21" s="43"/>
+      <c r="AP21" s="43"/>
+      <c r="AQ21" s="43"/>
+      <c r="AR21" s="43"/>
+      <c r="AS21" s="50"/>
+      <c r="AT21" s="50"/>
+      <c r="AU21" s="50"/>
+      <c r="AV21" s="50"/>
+      <c r="AW21" s="50"/>
+      <c r="AX21" s="50"/>
+      <c r="AY21" s="43"/>
+      <c r="AZ21" s="43"/>
+    </row>
+    <row r="22" spans="2:52" x14ac:dyDescent="0.3">
+      <c r="B22" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="D22" s="22"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="43"/>
+      <c r="K22" s="43"/>
+      <c r="L22" s="43"/>
+      <c r="M22" s="43"/>
+      <c r="N22" s="43"/>
+      <c r="O22" s="43"/>
+      <c r="P22" s="43"/>
+      <c r="Q22" s="43"/>
+      <c r="R22" s="43"/>
+      <c r="S22" s="43"/>
+      <c r="T22" s="43"/>
+      <c r="U22" s="43"/>
+      <c r="V22" s="43"/>
+      <c r="W22" s="43"/>
+      <c r="X22" s="43"/>
+      <c r="Y22" s="43"/>
+      <c r="Z22" s="43"/>
+      <c r="AA22" s="43"/>
+      <c r="AB22" s="43"/>
+      <c r="AC22" s="43"/>
+      <c r="AD22" s="43"/>
+      <c r="AE22" s="43"/>
+      <c r="AF22" s="43"/>
+      <c r="AG22" s="43"/>
+      <c r="AH22" s="43"/>
+      <c r="AI22" s="43"/>
+      <c r="AJ22" s="43"/>
+      <c r="AK22" s="43"/>
+      <c r="AL22" s="43"/>
+      <c r="AM22" s="43"/>
+      <c r="AN22" s="43"/>
+      <c r="AO22" s="43"/>
+      <c r="AP22" s="43"/>
+      <c r="AQ22" s="43"/>
+      <c r="AR22" s="43"/>
+      <c r="AS22" s="43"/>
+      <c r="AT22" s="43"/>
+      <c r="AU22" s="43"/>
+      <c r="AV22" s="43"/>
+      <c r="AW22" s="43"/>
+      <c r="AX22" s="43"/>
+      <c r="AY22" s="50"/>
+      <c r="AZ22" s="43"/>
+    </row>
+    <row r="23" spans="2:52" x14ac:dyDescent="0.3">
+      <c r="B23" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="C22" s="37" t="s">
-        <v>93</v>
-      </c>
-      <c r="D22" s="43" t="s">
-        <v>122</v>
-      </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="20"/>
-      <c r="L22" s="20"/>
-      <c r="M22" s="20"/>
-      <c r="N22" s="20"/>
-      <c r="O22" s="20"/>
-      <c r="P22" s="20"/>
-      <c r="Q22" s="20"/>
-      <c r="R22" s="20"/>
-      <c r="S22" s="20"/>
-      <c r="T22" s="20"/>
-      <c r="U22" s="20"/>
-      <c r="V22" s="20"/>
-      <c r="W22" s="20"/>
-      <c r="X22" s="20"/>
-      <c r="Y22" s="20"/>
-      <c r="Z22" s="20"/>
-      <c r="AA22" s="20"/>
-      <c r="AB22" s="20"/>
-      <c r="AC22" s="35"/>
-      <c r="AD22" s="35"/>
-      <c r="AE22" s="35"/>
-      <c r="AF22" s="35"/>
-      <c r="AG22" s="20"/>
-      <c r="AH22" s="20"/>
-      <c r="AI22" s="20"/>
-      <c r="AJ22" s="20"/>
-    </row>
-    <row r="23" spans="2:36" x14ac:dyDescent="0.3">
-      <c r="B23" s="27" t="s">
-        <v>91</v>
-      </c>
-      <c r="C23" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="D23" s="23"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="22"/>
       <c r="E23" s="2"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="22"/>
-      <c r="K23" s="22"/>
-      <c r="L23" s="22"/>
-      <c r="M23" s="22"/>
-      <c r="N23" s="22"/>
-      <c r="O23" s="22"/>
-      <c r="P23" s="22"/>
-      <c r="Q23" s="22"/>
-      <c r="R23" s="22"/>
-      <c r="S23" s="22"/>
-      <c r="T23" s="22"/>
-      <c r="U23" s="22"/>
-      <c r="V23" s="22"/>
-      <c r="W23" s="22"/>
-      <c r="X23" s="22"/>
-      <c r="Y23" s="22"/>
-      <c r="Z23" s="22"/>
-      <c r="AA23" s="22"/>
-      <c r="AB23" s="22"/>
-      <c r="AC23" s="35"/>
-      <c r="AD23" s="35"/>
-      <c r="AE23" s="35"/>
-      <c r="AF23" s="35"/>
-      <c r="AG23" s="35"/>
-      <c r="AH23" s="30"/>
-      <c r="AI23" s="30"/>
-      <c r="AJ23" s="22"/>
-    </row>
-    <row r="24" spans="2:36" x14ac:dyDescent="0.3">
-      <c r="B24" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="C24" s="28"/>
-      <c r="D24" s="23"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+      <c r="V23" s="2"/>
+      <c r="W23" s="2"/>
+      <c r="X23" s="2"/>
+      <c r="Y23" s="2"/>
+      <c r="Z23" s="2"/>
+      <c r="AA23" s="2"/>
+      <c r="AB23" s="2"/>
+      <c r="AC23" s="2"/>
+      <c r="AD23" s="2"/>
+      <c r="AE23" s="2"/>
+      <c r="AF23" s="2"/>
+      <c r="AG23" s="2"/>
+      <c r="AH23" s="43"/>
+      <c r="AI23" s="43"/>
+      <c r="AJ23" s="43"/>
+      <c r="AK23" s="43"/>
+      <c r="AL23" s="43"/>
+      <c r="AM23" s="43"/>
+      <c r="AN23" s="43"/>
+      <c r="AO23" s="43"/>
+      <c r="AP23" s="43"/>
+      <c r="AQ23" s="43"/>
+      <c r="AR23" s="43"/>
+      <c r="AS23" s="43"/>
+      <c r="AT23" s="43"/>
+      <c r="AU23" s="43"/>
+      <c r="AV23" s="43"/>
+      <c r="AW23" s="43"/>
+      <c r="AX23" s="43"/>
+      <c r="AY23" s="43"/>
+      <c r="AZ23" s="43"/>
+    </row>
+    <row r="24" spans="2:52" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B24" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="D24" s="39" t="s">
+        <v>137</v>
+      </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
+      <c r="I24" s="28"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="28"/>
+      <c r="L24" s="28"/>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
@@ -2216,27 +2726,43 @@
       <c r="W24" s="2"/>
       <c r="X24" s="2"/>
       <c r="Y24" s="2"/>
-      <c r="Z24" s="2"/>
-      <c r="AA24" s="2"/>
-      <c r="AB24" s="2"/>
-      <c r="AC24" s="2"/>
-      <c r="AD24" s="2"/>
-      <c r="AE24" s="2"/>
-      <c r="AF24" s="2"/>
-      <c r="AG24" s="2"/>
-      <c r="AH24" s="2"/>
-      <c r="AI24" s="2"/>
-      <c r="AJ24" s="2"/>
-    </row>
-    <row r="25" spans="2:36" x14ac:dyDescent="0.3">
-      <c r="B25" s="27" t="s">
-        <v>67</v>
-      </c>
-      <c r="C25" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="D25" s="23" t="s">
-        <v>144</v>
+      <c r="Z24" s="57"/>
+      <c r="AA24" s="57"/>
+      <c r="AB24" s="57"/>
+      <c r="AC24" s="57"/>
+      <c r="AD24" s="57"/>
+      <c r="AE24" s="57"/>
+      <c r="AF24" s="57"/>
+      <c r="AG24" s="57"/>
+      <c r="AH24" s="43"/>
+      <c r="AI24" s="43"/>
+      <c r="AJ24" s="43"/>
+      <c r="AK24" s="43"/>
+      <c r="AL24" s="43"/>
+      <c r="AM24" s="43"/>
+      <c r="AN24" s="43"/>
+      <c r="AO24" s="43"/>
+      <c r="AP24" s="43"/>
+      <c r="AQ24" s="43"/>
+      <c r="AR24" s="43"/>
+      <c r="AS24" s="43"/>
+      <c r="AT24" s="43"/>
+      <c r="AU24" s="43"/>
+      <c r="AV24" s="43"/>
+      <c r="AW24" s="43"/>
+      <c r="AX24" s="43"/>
+      <c r="AY24" s="43"/>
+      <c r="AZ24" s="43"/>
+    </row>
+    <row r="25" spans="2:52" x14ac:dyDescent="0.3">
+      <c r="B25" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="D25" s="41" t="s">
+        <v>118</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
@@ -2259,66 +2785,275 @@
       <c r="W25" s="2"/>
       <c r="X25" s="2"/>
       <c r="Y25" s="2"/>
-      <c r="Z25" s="30"/>
-      <c r="AA25" s="30"/>
-      <c r="AB25" s="30"/>
-      <c r="AC25" s="30"/>
-      <c r="AD25" s="30"/>
-      <c r="AE25" s="30"/>
-      <c r="AF25" s="30"/>
-      <c r="AG25" s="30"/>
-      <c r="AH25" s="30"/>
-      <c r="AI25" s="30"/>
-      <c r="AJ25" s="30"/>
-    </row>
-    <row r="26" spans="2:36" x14ac:dyDescent="0.3">
-      <c r="B26" s="27" t="s">
-        <v>125</v>
-      </c>
-      <c r="C26" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="D26" s="41" t="s">
-        <v>136</v>
-      </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
-      <c r="O26" s="2"/>
-      <c r="P26" s="2"/>
-      <c r="Q26" s="2"/>
-      <c r="R26" s="2"/>
-      <c r="S26" s="2"/>
-      <c r="T26" s="2"/>
-      <c r="U26" s="2"/>
-      <c r="V26" s="2"/>
-      <c r="W26" s="2"/>
-      <c r="X26" s="2"/>
-      <c r="Y26" s="2"/>
-      <c r="Z26" s="30"/>
-      <c r="AA26" s="30"/>
-      <c r="AB26" s="30"/>
-      <c r="AC26" s="30"/>
-      <c r="AD26" s="30"/>
-      <c r="AE26" s="30"/>
-      <c r="AF26" s="30"/>
-      <c r="AG26" s="30"/>
-      <c r="AH26" s="30"/>
-      <c r="AI26" s="30"/>
-      <c r="AJ26" s="30"/>
+      <c r="Z25" s="57"/>
+      <c r="AA25" s="57"/>
+      <c r="AB25" s="57"/>
+      <c r="AC25" s="57"/>
+      <c r="AD25" s="57"/>
+      <c r="AE25" s="57"/>
+      <c r="AF25" s="57"/>
+      <c r="AG25" s="57"/>
+      <c r="AH25" s="43"/>
+      <c r="AI25" s="43"/>
+      <c r="AJ25" s="43"/>
+      <c r="AK25" s="43"/>
+      <c r="AL25" s="43"/>
+      <c r="AM25" s="43"/>
+      <c r="AN25" s="43"/>
+      <c r="AO25" s="43"/>
+      <c r="AP25" s="43"/>
+      <c r="AQ25" s="43"/>
+      <c r="AR25" s="43"/>
+      <c r="AS25" s="43"/>
+      <c r="AT25" s="43"/>
+      <c r="AU25" s="43"/>
+      <c r="AV25" s="43"/>
+      <c r="AW25" s="43"/>
+      <c r="AX25" s="43"/>
+      <c r="AY25" s="43"/>
+      <c r="AZ25" s="43"/>
+    </row>
+    <row r="26" spans="2:52" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="52" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="53" t="s">
+        <v>161</v>
+      </c>
+      <c r="D26" s="54" t="s">
+        <v>138</v>
+      </c>
+      <c r="E26" s="55"/>
+      <c r="F26" s="55"/>
+      <c r="G26" s="55"/>
+      <c r="H26" s="55"/>
+      <c r="I26" s="55"/>
+      <c r="J26" s="55"/>
+      <c r="K26" s="55"/>
+      <c r="L26" s="55"/>
+      <c r="M26" s="55"/>
+      <c r="N26" s="55"/>
+      <c r="O26" s="55"/>
+      <c r="P26" s="55"/>
+      <c r="Q26" s="55"/>
+      <c r="R26" s="55"/>
+      <c r="S26" s="55"/>
+      <c r="T26" s="55"/>
+      <c r="U26" s="55"/>
+      <c r="V26" s="55"/>
+      <c r="W26" s="55"/>
+      <c r="X26" s="55"/>
+      <c r="Y26" s="55"/>
+      <c r="Z26" s="56"/>
+      <c r="AA26" s="56"/>
+      <c r="AB26" s="56"/>
+      <c r="AC26" s="56"/>
+      <c r="AD26" s="56"/>
+      <c r="AE26" s="56"/>
+      <c r="AF26" s="56"/>
+      <c r="AG26" s="56"/>
+      <c r="AH26" s="56"/>
+      <c r="AI26" s="56"/>
+      <c r="AJ26" s="56"/>
+      <c r="AK26" s="56"/>
+      <c r="AL26" s="56"/>
+      <c r="AM26" s="56"/>
+      <c r="AN26" s="56"/>
+      <c r="AO26" s="56"/>
+      <c r="AP26" s="56"/>
+      <c r="AQ26" s="56"/>
+      <c r="AR26" s="56"/>
+      <c r="AS26" s="56"/>
+      <c r="AT26" s="56"/>
+      <c r="AU26" s="56"/>
+      <c r="AV26" s="56"/>
+      <c r="AW26" s="56"/>
+      <c r="AX26" s="56"/>
+      <c r="AY26" s="56"/>
+      <c r="AZ26" s="56"/>
+    </row>
+    <row r="27" spans="2:52" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B27" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="C27" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="D27" s="58" t="s">
+        <v>172</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2"/>
+      <c r="U27" s="2"/>
+      <c r="V27" s="2"/>
+      <c r="W27" s="2"/>
+      <c r="X27" s="2"/>
+      <c r="Y27" s="2"/>
+      <c r="Z27" s="28"/>
+      <c r="AA27" s="28"/>
+      <c r="AB27" s="28"/>
+      <c r="AC27" s="28"/>
+      <c r="AD27" s="28"/>
+      <c r="AE27" s="28"/>
+      <c r="AF27" s="28"/>
+      <c r="AG27" s="28"/>
+      <c r="AH27" s="28"/>
+      <c r="AI27" s="28"/>
+      <c r="AJ27" s="28"/>
+      <c r="AK27" s="28"/>
+      <c r="AL27" s="28"/>
+      <c r="AM27" s="28"/>
+      <c r="AN27" s="28"/>
+      <c r="AO27" s="28"/>
+      <c r="AP27" s="28"/>
+      <c r="AQ27" s="28"/>
+      <c r="AR27" s="28"/>
+      <c r="AS27" s="28"/>
+      <c r="AT27" s="28"/>
+      <c r="AU27" s="28"/>
+      <c r="AV27" s="28"/>
+      <c r="AW27" s="28"/>
+      <c r="AX27" s="28"/>
+      <c r="AY27" s="28"/>
+      <c r="AZ27" s="28"/>
+    </row>
+    <row r="28" spans="2:52" x14ac:dyDescent="0.3">
+      <c r="B28" s="26" t="s">
+        <v>166</v>
+      </c>
+      <c r="C28" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="D28" s="23"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2"/>
+      <c r="S28" s="2"/>
+      <c r="T28" s="2"/>
+      <c r="U28" s="2"/>
+      <c r="V28" s="2"/>
+      <c r="W28" s="2"/>
+      <c r="X28" s="2"/>
+      <c r="Y28" s="2"/>
+      <c r="Z28" s="2"/>
+      <c r="AA28" s="2"/>
+      <c r="AB28" s="2"/>
+      <c r="AC28" s="28"/>
+      <c r="AD28" s="28"/>
+      <c r="AE28" s="28"/>
+      <c r="AF28" s="28"/>
+      <c r="AG28" s="2"/>
+      <c r="AH28" s="2"/>
+      <c r="AI28" s="2"/>
+      <c r="AJ28" s="2"/>
+      <c r="AK28" s="43"/>
+      <c r="AL28" s="43"/>
+      <c r="AM28" s="43"/>
+      <c r="AN28" s="43"/>
+      <c r="AO28" s="43"/>
+      <c r="AP28" s="43"/>
+      <c r="AQ28" s="43"/>
+      <c r="AR28" s="43"/>
+      <c r="AS28" s="43"/>
+      <c r="AT28" s="43"/>
+      <c r="AU28" s="43"/>
+      <c r="AV28" s="43"/>
+      <c r="AW28" s="43"/>
+      <c r="AX28" s="43"/>
+      <c r="AY28" s="43"/>
+      <c r="AZ28" s="43"/>
+    </row>
+    <row r="29" spans="2:52" x14ac:dyDescent="0.3">
+      <c r="B29" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="C29" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="D29" s="23"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="2"/>
+      <c r="S29" s="2"/>
+      <c r="T29" s="2"/>
+      <c r="U29" s="2"/>
+      <c r="V29" s="2"/>
+      <c r="W29" s="2"/>
+      <c r="X29" s="2"/>
+      <c r="Y29" s="2"/>
+      <c r="Z29" s="2"/>
+      <c r="AA29" s="2"/>
+      <c r="AB29" s="2"/>
+      <c r="AC29" s="2"/>
+      <c r="AD29" s="2"/>
+      <c r="AE29" s="2"/>
+      <c r="AF29" s="2"/>
+      <c r="AG29" s="2"/>
+      <c r="AH29" s="2"/>
+      <c r="AI29" s="2"/>
+      <c r="AJ29" s="2"/>
+      <c r="AK29" s="49"/>
+      <c r="AL29" s="49"/>
+      <c r="AM29" s="49"/>
+      <c r="AN29" s="49"/>
+      <c r="AO29" s="49"/>
+      <c r="AP29" s="49"/>
+      <c r="AQ29" s="49"/>
+      <c r="AR29" s="49"/>
+      <c r="AS29" s="49"/>
+      <c r="AT29" s="49"/>
+      <c r="AU29" s="49"/>
+      <c r="AV29" s="49"/>
+      <c r="AW29" s="49"/>
+      <c r="AX29" s="49"/>
+      <c r="AY29" s="49"/>
+      <c r="AZ29" s="50"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="14">
+    <mergeCell ref="AK7:AN7"/>
+    <mergeCell ref="AO7:AR7"/>
+    <mergeCell ref="AS7:AV7"/>
+    <mergeCell ref="AW7:AZ7"/>
+    <mergeCell ref="Y6:AZ6"/>
     <mergeCell ref="AG7:AJ7"/>
     <mergeCell ref="E6:X6"/>
-    <mergeCell ref="Y6:AJ6"/>
     <mergeCell ref="AC7:AF7"/>
     <mergeCell ref="E7:H7"/>
     <mergeCell ref="I7:L7"/>
@@ -2388,13 +3123,13 @@
     </row>
     <row r="7" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B7" s="14" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>32</v>
@@ -2402,13 +3137,13 @@
     </row>
     <row r="8" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B8" s="14" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>45</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="E8" s="14"/>
     </row>
@@ -2417,10 +3152,10 @@
         <v>21</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>32</v>
@@ -2428,27 +3163,27 @@
     </row>
     <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="9" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C10" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>159</v>
-      </c>
       <c r="E10" s="9" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="31" t="s">
-        <v>86</v>
+      <c r="D11" s="29" t="s">
+        <v>84</v>
       </c>
       <c r="E11" s="14" t="s">
         <v>32</v>
@@ -2456,53 +3191,53 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" s="14" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>45</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B13" s="38" t="s">
-        <v>105</v>
-      </c>
-      <c r="C13" s="39" t="s">
+      <c r="B13" s="36" t="s">
+        <v>101</v>
+      </c>
+      <c r="C13" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="40" t="s">
-        <v>139</v>
-      </c>
-      <c r="E13" s="38" t="s">
+      <c r="D13" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="E13" s="36" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B14" s="11" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="33" t="s">
-        <v>138</v>
+      <c r="D14" s="31" t="s">
+        <v>133</v>
       </c>
       <c r="E14" s="11"/>
     </row>
     <row r="15" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B15" s="11" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="E15" s="11" t="s">
         <v>32</v>
@@ -2513,38 +3248,38 @@
         <v>29</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B17" s="38" t="s">
-        <v>128</v>
-      </c>
-      <c r="C17" s="39" t="s">
+      <c r="B17" s="36" t="s">
+        <v>123</v>
+      </c>
+      <c r="C17" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="D17" s="38" t="s">
-        <v>137</v>
-      </c>
-      <c r="E17" s="38" t="s">
+      <c r="D17" s="36" t="s">
+        <v>132</v>
+      </c>
+      <c r="E17" s="36" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="18" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B18" s="11" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="E18" s="11" t="s">
         <v>32</v>
@@ -2552,13 +3287,13 @@
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="11" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>45</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="E19" s="11" t="s">
         <v>32</v>
@@ -2566,13 +3301,13 @@
     </row>
     <row r="20" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B20" s="11" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>45</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="E20" s="11" t="s">
         <v>32</v>
@@ -2580,13 +3315,13 @@
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="11" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>45</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E21" s="11" t="s">
         <v>32</v>
@@ -2594,13 +3329,13 @@
     </row>
     <row r="22" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B22" s="11" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>45</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E22" s="11" t="s">
         <v>32</v>
@@ -2608,13 +3343,13 @@
     </row>
     <row r="23" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B23" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="44" t="s">
-        <v>145</v>
+      <c r="D23" s="42" t="s">
+        <v>139</v>
       </c>
       <c r="E23" s="11" t="s">
         <v>32</v>
@@ -2622,13 +3357,13 @@
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" s="30" t="s">
         <v>96</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="D24" s="32" t="s">
-        <v>100</v>
       </c>
       <c r="E24" s="11" t="s">
         <v>32</v>
@@ -2636,13 +3371,13 @@
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="11" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C25" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="34" t="s">
-        <v>126</v>
+      <c r="D25" s="32" t="s">
+        <v>121</v>
       </c>
       <c r="E25" s="11" t="s">
         <v>32</v>
@@ -2650,13 +3385,13 @@
     </row>
     <row r="26" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B26" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="D26" s="33" t="s">
-        <v>101</v>
+        <v>80</v>
+      </c>
+      <c r="D26" s="31" t="s">
+        <v>97</v>
       </c>
       <c r="E26" s="11" t="s">
         <v>32</v>
@@ -2664,69 +3399,69 @@
     </row>
     <row r="27" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B27" s="11" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="D27" s="33" t="s">
-        <v>120</v>
+        <v>100</v>
+      </c>
+      <c r="D27" s="31" t="s">
+        <v>116</v>
       </c>
       <c r="E27" s="11" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="28" spans="2:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="B28" s="38" t="s">
-        <v>112</v>
-      </c>
-      <c r="C28" s="39" t="s">
+      <c r="B28" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="C28" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="D28" s="40" t="s">
-        <v>113</v>
-      </c>
-      <c r="E28" s="38" t="s">
+      <c r="D28" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="E28" s="36" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="29" spans="2:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B29" s="11" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C29" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D29" s="33" t="s">
-        <v>111</v>
+      <c r="D29" s="31" t="s">
+        <v>107</v>
       </c>
       <c r="E29" s="11" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="30" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B30" s="38" t="s">
-        <v>108</v>
-      </c>
-      <c r="C30" s="39" t="s">
-        <v>109</v>
-      </c>
-      <c r="D30" s="40" t="s">
-        <v>110</v>
-      </c>
-      <c r="E30" s="38" t="s">
+      <c r="B30" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="C30" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="D30" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="E30" s="36" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="31" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B31" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="D31" s="32" t="s">
-        <v>102</v>
+        <v>80</v>
+      </c>
+      <c r="D31" s="30" t="s">
+        <v>98</v>
       </c>
       <c r="E31" s="11" t="s">
         <v>32</v>
@@ -2734,13 +3469,13 @@
     </row>
     <row r="32" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B32" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="D32" s="32" t="s">
-        <v>97</v>
+        <v>79</v>
+      </c>
+      <c r="D32" s="30" t="s">
+        <v>93</v>
       </c>
       <c r="E32" s="11" t="s">
         <v>32</v>
@@ -2782,35 +3517,35 @@
         <v>34</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E35" s="11" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="36" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B36" s="38" t="s">
+      <c r="B36" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="C36" s="39" t="s">
+      <c r="C36" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="D36" s="38" t="s">
-        <v>78</v>
-      </c>
-      <c r="E36" s="38" t="s">
+      <c r="D36" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="E36" s="36" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="37" spans="2:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B37" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C37" s="12" t="s">
         <v>44</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E37" s="11" t="s">
         <v>32</v>
@@ -2824,35 +3559,35 @@
         <v>44</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E38" s="11" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B39" s="38" t="s">
+      <c r="B39" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="C39" s="39" t="s">
+      <c r="C39" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="D39" s="38" t="s">
-        <v>127</v>
-      </c>
-      <c r="E39" s="38" t="s">
+      <c r="D39" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="E39" s="36" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="40" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B40" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C40" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D40" s="32" t="s">
-        <v>98</v>
+      <c r="D40" s="30" t="s">
+        <v>94</v>
       </c>
       <c r="E40" s="11" t="s">
         <v>32</v>
@@ -2866,7 +3601,7 @@
         <v>30</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E41" s="11" t="s">
         <v>32</v>
@@ -2880,7 +3615,7 @@
         <v>30</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E42" s="11" t="s">
         <v>32</v>
@@ -2894,23 +3629,23 @@
         <v>30</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E43" s="11" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="44" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B44" s="38" t="s">
+      <c r="B44" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="C44" s="39" t="s">
+      <c r="C44" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="D44" s="38" t="s">
+      <c r="D44" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="E44" s="38" t="s">
+      <c r="E44" s="36" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2922,7 +3657,7 @@
         <v>43</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E45" s="11" t="s">
         <v>32</v>
@@ -2930,12 +3665,12 @@
     </row>
     <row r="46" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B46" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C46" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D46" s="34" t="s">
+      <c r="D46" s="32" t="s">
         <v>35</v>
       </c>
       <c r="E46" s="11" t="s">
@@ -2944,13 +3679,13 @@
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B47" s="11" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C47" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D47" s="34" t="s">
-        <v>75</v>
+      <c r="D47" s="32" t="s">
+        <v>73</v>
       </c>
       <c r="E47" s="11" t="s">
         <v>32</v>
@@ -2959,7 +3694,7 @@
   </sheetData>
   <autoFilter ref="A6:G44" xr:uid="{2C350AE8-6BD8-4071-BE8D-EB446D52B86B}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:G47">
-      <sortCondition sortBy="cellColor" ref="B6:B44" dxfId="1"/>
+      <sortCondition sortBy="cellColor" ref="B6:B44" dxfId="0"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2991,7 +3726,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -3062,13 +3797,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12" s="18" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C12" s="19">
         <v>1</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>